<commit_message>
1. Finish the sql command of inserting, except Transaction and TransactionFood. 2. Revise the database design to make it more reasonable.
</commit_message>
<xml_diff>
--- a/database_design/database_design.xlsx
+++ b/database_design/database_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\108-1\database\project\database_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27AF628-E3CB-4A66-B88F-4CAAE883C575}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B785D4B-0FFC-417E-86B4-5F124DD90166}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{0450CEB7-846B-49EA-9E7B-6AB4BD7DCD46}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>User</t>
   </si>
@@ -60,15 +60,6 @@
     <t>supportedPlatform</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>CID</t>
-  </si>
-  <si>
-    <t>Cname</t>
-  </si>
-  <si>
     <t>Food</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
     <t>RestaurantCategory</t>
   </si>
   <si>
-    <t>ResaurantFood</t>
-  </si>
-  <si>
     <t>acount</t>
   </si>
   <si>
@@ -169,6 +157,9 @@
   </si>
   <si>
     <t>discount_shippingFee</t>
+  </si>
+  <si>
+    <t>CName</t>
   </si>
 </sst>
 </file>
@@ -224,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -285,17 +276,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -323,7 +303,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -341,9 +321,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -356,6 +335,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -672,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D228CC6-8A87-4349-861A-81101189E755}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -686,22 +668,22 @@
     <col min="6" max="6" width="18.09765625" customWidth="1"/>
     <col min="7" max="7" width="13.19921875" customWidth="1"/>
     <col min="8" max="8" width="11.09765625" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="9.3984375" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="H1" s="7"/>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -712,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -721,25 +703,25 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
@@ -749,7 +731,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -757,7 +739,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -767,81 +749,82 @@
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
+      <c r="A10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -852,7 +835,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>5</v>
@@ -860,141 +843,113 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2"/>
+      <c r="A16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="4"/>
+      <c r="A19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>37</v>
+      <c r="A20" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>15</v>
+      <c r="A23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>16</v>
+      <c r="G23" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>